<commit_message>
Documented grouping mismatch CBB/Observation
</commit_message>
<xml_diff>
--- a/Supporting documents/AlcoholUse.xlsx
+++ b/Supporting documents/AlcoholUse.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28130"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahenket/Development/GitHub/Nictiz/MedMij-DSTU2/Supporting documents/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12600"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17480"/>
   </bookViews>
   <sheets>
     <sheet name="AlcoholGebruik" sheetId="1" r:id="rId1"/>
     <sheet name="AlcoholGebruikStatusCodelijst" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="50">
   <si>
     <t xml:space="preserve"># </t>
   </si>
@@ -174,12 +187,15 @@
   <si>
     <t>Set constrains on references to  only ZIB profiles for new basedOn element and context element in the nl-core-observation</t>
   </si>
+  <si>
+    <t>There is no option to keep the three propoerties together, so for every combination of AlcoholUseStatus/UsageObservation you need a new instance of Observation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -481,7 +497,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
@@ -566,46 +582,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Neutral 2" xfId="2"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -618,7 +633,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -660,12 +675,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -695,12 +710,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -907,35 +922,35 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:B23"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="9.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" customWidth="1"/>
-    <col min="9" max="9" width="25.85546875" customWidth="1"/>
-    <col min="10" max="10" width="36.42578125" customWidth="1"/>
-    <col min="11" max="11" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.796875" customWidth="1"/>
+    <col min="4" max="4" width="18.19921875" customWidth="1"/>
+    <col min="5" max="5" width="6.3984375" customWidth="1"/>
+    <col min="6" max="6" width="9.796875" customWidth="1"/>
+    <col min="7" max="7" width="7.796875" customWidth="1"/>
+    <col min="8" max="8" width="9.796875" customWidth="1"/>
+    <col min="9" max="9" width="25.796875" customWidth="1"/>
+    <col min="10" max="10" width="36.3984375" customWidth="1"/>
+    <col min="11" max="11" width="59.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
       <c r="I1" s="2" t="s">
         <v>2</v>
       </c>
@@ -946,32 +961,32 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="24" customHeight="1">
+    <row r="2" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="41"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="40"/>
       <c r="J2" s="5" t="s">
         <v>16</v>
       </c>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:11" ht="15">
+    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>1</v>
       </c>
       <c r="B3" s="7"/>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="42"/>
+      <c r="D3" s="41"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8" t="s">
         <v>20</v>
@@ -986,15 +1001,15 @@
       </c>
       <c r="K3" s="23"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
         <v>2</v>
       </c>
       <c r="B4" s="11"/>
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="43"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12" t="s">
         <v>21</v>
@@ -1009,24 +1024,26 @@
       </c>
       <c r="K4" s="21"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" ht="39" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
         <v>3</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="43"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14"/>
       <c r="J5" s="27"/>
-      <c r="K5" s="20"/>
-    </row>
-    <row r="6" spans="1:11" ht="15">
+      <c r="K5" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="10">
         <v>4</v>
       </c>
@@ -1049,7 +1066,7 @@
       </c>
       <c r="K6" s="28"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="10">
         <v>5</v>
       </c>
@@ -1072,7 +1089,7 @@
       </c>
       <c r="K7" s="21"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="15">
         <v>6</v>
       </c>
@@ -1095,37 +1112,37 @@
       </c>
       <c r="K8" s="19"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K10" s="26"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75">
-      <c r="A12" s="34" t="s">
+    <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
       <c r="I13" s="2" t="s">
         <v>2</v>
       </c>
@@ -1136,32 +1153,32 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15">
+    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="41"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="40"/>
       <c r="J14" s="5" t="s">
         <v>16</v>
       </c>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>1</v>
       </c>
       <c r="B15" s="7"/>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="42"/>
+      <c r="D15" s="41"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8" t="s">
         <v>20</v>
@@ -1171,20 +1188,20 @@
       <c r="I15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J15" s="44" t="s">
+      <c r="J15" s="33" t="s">
         <v>47</v>
       </c>
       <c r="K15" s="29"/>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="10">
         <v>2</v>
       </c>
       <c r="B16" s="11"/>
-      <c r="C16" s="43" t="s">
+      <c r="C16" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="43"/>
+      <c r="D16" s="34"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12" t="s">
         <v>21</v>
@@ -1199,24 +1216,26 @@
       </c>
       <c r="K16" s="30"/>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" ht="39" x14ac:dyDescent="0.2">
       <c r="A17" s="10">
         <v>3</v>
       </c>
       <c r="B17" s="11"/>
-      <c r="C17" s="43" t="s">
+      <c r="C17" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="43"/>
+      <c r="D17" s="34"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
       <c r="H17" s="13"/>
       <c r="I17" s="14"/>
       <c r="J17" s="27"/>
-      <c r="K17" s="32"/>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="K17" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="10">
         <v>4</v>
       </c>
@@ -1239,7 +1258,7 @@
       </c>
       <c r="K18" s="30"/>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="10">
         <v>5</v>
       </c>
@@ -1262,7 +1281,7 @@
       </c>
       <c r="K19" s="30"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="15">
         <v>6</v>
       </c>
@@ -1285,12 +1304,12 @@
       </c>
       <c r="K20" s="31"/>
     </row>
-    <row r="22" spans="1:11">
-      <c r="B22" s="33" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B22" s="32" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>48</v>
       </c>
@@ -1322,16 +1341,16 @@
       <selection activeCell="B2" sqref="B2:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.19921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>24</v>
       </c>
@@ -1339,7 +1358,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:6">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>26</v>
       </c>
@@ -1356,7 +1375,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>31</v>
       </c>
@@ -1373,7 +1392,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>35</v>
       </c>
@@ -1390,7 +1409,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>37</v>
       </c>
@@ -1407,7 +1426,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>39</v>
       </c>

</xml_diff>